<commit_message>
features not working right :(
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="1000">
   <si>
     <t>SKU</t>
   </si>
@@ -1219,6 +1219,1806 @@
   </si>
   <si>
     <t>http://cby.alsoactebis.com/cop/product/2395600/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-F33E1-100-02-12</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3871888/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-F36E1-284-02-36</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3868330/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>brother-4977766787895</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3125199/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>bosch telecom-4242002718743</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3626426/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>assmann-4016032336648</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/2834221/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>ea-5030949123879</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/4264165/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC4-10-FNAC1-209-01-12</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/4028399/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>4world-5908214360338</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3588808/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>xerox-0095205845594</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3627873/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>xerox-0095205740219</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/2330551/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>hp-0193015599352</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3092298/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>epson-8715946524177</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/1919832/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>techly-8051128101768</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3642005/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>gembird-8716309100991</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3641815/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>lenovo-0194632482072</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3923394/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>natec-5901969400861</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3594344/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>mikrotik-5903148913087</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3616437/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-FVMUL-231-02-12</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3895683/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>lexmark-0734646586290</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/2521870/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>lanberg-5901969428087</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3904789/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>hp-0192018667501</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3073839/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>tracer-5907512863176</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3610641/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>lanberg-5901969423563</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3765481/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>transcend-0760557817543</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/1584494/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>activision-5030917146251</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3647284/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>asus-4718017734714</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3921074/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-W04HE-212-02-12</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/4028543/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>apacer-4712389902962</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3598735/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>asrock-4710483933721</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/4143251/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>ea-5035226121609</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3584556/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>gnnetcom-5706991023305</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3845302/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>netgear-0606449102499</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/2353481/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>acer-4713883884235</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3897788/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>tplink-6935364050696</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/1881354/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>canon-4960999904818</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/1915606/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>lanberg-5901969415940</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3635508/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>mikrotik-4752224002310</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/4153699/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-F40FG-179-02-12</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3894294/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>philips-8712581759162</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3755749/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>teamg-0765441632240</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3601049/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FPC-VM-100-UG</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3872522/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>asus-4711081469698</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/4359576/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>gembird-8716309074049</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3597717/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-00240-950-02-12</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/2692944/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>intel-0675901759632</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3499406/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>hp-4573257520547</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/2510120/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>gnnetcom-5706991019971</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/2609200/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>oki-5031713067351</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/2643600/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>synology-4711174720293</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/2591594/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>samsung-8801643264130</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3057810/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>lenovo-0192330831130</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3026258/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>zalman-CNPS4X</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3746407/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>gembird-8716309074056</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3597719/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>assmann-4016032433699</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/2989726/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>hp-0848412014358</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/2320276/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC3-10-M3004-248-02-60</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3872431/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>asus-4718017666046</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3864666/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>wd-0718037868738</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3580305/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>epson-8715946333205</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/1311753/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>samsung-8801643644512</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3372887/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>gembird-8716309094016</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3641168/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>lanberg-5901969404913</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3635048/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-D4H1E-247-02-12</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/4029013/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-00307-817-02-36</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3894912/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-W248E-247-02-36</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3869513/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>hama-4047443311580</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/2664222/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>qoltec-5901878500508</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3653757/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>samsung-8806092001992</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/4092023/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>hp-H9FX2E</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3068859/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>tplink-6935364084745</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3387168/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>cecotec-8435484054393</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/4071260/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>wd-0718037856773</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/2826493/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>philips-8712581761868</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/4037328/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>lanberg-5901969414486</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3635339/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>siliconpower-4713436130017</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3841383/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>hp-0889894377920</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/2479192/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-0081F-319-02-12</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/4028904/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>icybox-4250078162520</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3637915/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>lanberg-5901969427905</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3904773/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>natec-5908257123235</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3596919/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>samsung-8806090312465</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3865302/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>listan-4260052184462</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3531961/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>qoltec-5901878515182</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3655670/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>transcend-0760557843603</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3397417/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>pny-711-VPC022-P2CMI36</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/2924965/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>unitek-4894160021779</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3645222/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>assmann-4016032455110</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3432971/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>microsoft-0885370249019</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/1635675/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>epson-8715946688749</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/4060166/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>qoltec-5901878522210</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3657099/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-L02KE-247-02-12</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/2724834/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>netgear-0606449064131</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/1531835/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>coolermaster-4719512054116</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/2713974/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>dicota-7332752004801</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3634559/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fellowes-0077511938047</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/2643132/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>zotac-4895173608872</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/2514085/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>gembird-8716309078689</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3597966/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FCC-10-FSM97-248-02-60</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3872830/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>kingston-0740617291360</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3394263/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>tplink-6935364092740</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/2433903/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>gembird-8716309088114</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3604960/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>canon-4960999675329</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/1624627/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>delock-4043619834334</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/2924446/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>bluebaum-0878615024281</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/2769842/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-F11E1-108-02-12</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3870633/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>razer-8886419344940</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3587720/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>samsung-8806092238268</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/4138048/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>gembird-8716309068741</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3641633/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>samsung-8806088880174</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/2916819/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>gembird-8716309029209</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3597668/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>oki-5031713071013</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3422983/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>a-data-4713218469458</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3155382/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>assmann-4016032249153</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/1506839/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-I30EN-284-02-12</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3873223/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>samsung-8801643110864</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/2968879/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>a-data-4713218469144</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3846228/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>vertiv-4YSLV-LCD</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/1879159/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-W248D-210-02-12</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3869499/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>ubiquiti-0810354022265</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3616173/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>delock-4043619852338</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/2874084/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>gnnetcom-5706991017281</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/2321459/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>a-data-4718050602308</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/1641070/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-AP024-247-02-12</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3111158/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>dlink-0790069456596</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/4153977/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>netgear-0606449149586</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/4031880/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>qoltec-5901878516370</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3656641/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>canon-4549292057881</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/2549344/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-F11HE-284-02-12</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3870360/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>dicota-7640158669839</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/4120508/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>siliconpower-4712702629408</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3589416/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>lanberg-5901969430400</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/4326072/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>leitz-0636638006291</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/1209358/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-0080E-131-02-60</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/2979817/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>asus-4718017749688</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3899499/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-VVM08-248-02-60</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3869527/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-00098-159-02-12</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/2982731/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-W040F-131-02-60</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/4028978/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>corsair-0840006603641</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/4155335/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>arctic-4895213701907</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3751547/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>hp-H28W5E</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/4259672/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-L02KE-211-02-12</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3865523/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>intracom-0766623164580</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3348276/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-F433F-210-02-12</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3895605/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>epson-0010343819788</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/1009342/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>hp-0193015506459</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3420417/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC5-10-FSM98-149-02-36</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3872730/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-7K3E3-210-02-12</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3868640/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>lanberg-5901969414004</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3635318/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>powerw-4260074981179</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3596219/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>lanberg-5901969413496</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3635273/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FCD-10-FSM99-240-02-36</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3872957/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>verbatim-0023942435525</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/2330530/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-00119-131-02-60</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/2982826/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>eaton-0743172045157</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/2006714/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>raidsonic-4250078184751</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/1802291/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>epson-8715946639499</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/2891650/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-G30EN-131-02-12</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/2984927/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>lanberg-5901969424607</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3904804/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>garett-5903246285000</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3850282/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>gembird-8716309093040</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3640744/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>lg-8806098289509</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3141691/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>gembird-8716309107976</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3643528/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>xerox-0095205860160</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/2873872/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>logilink-4052792045673</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3614306/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>defender-4714033631112</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/2500229/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>greencell-5903317225683</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3601628/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>leitz-0085896625605</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/1415382/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>assmann-4016032469971</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/4245771/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-X0CME-608-02-36</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3865953/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>newstar-8717371444525</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/2157452/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>hp-0195122634100</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3904885/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>assmann-4016032458104</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3932135/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>intel-5032037102766</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/2916250/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-0080D-284-02-12</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3868265/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>amd-0730143309165</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3024123/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>asus-4716659922230</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/2327145/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>hp-0195122907846</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/4027961/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>epson-8715946687414</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/4198588/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>netrack-5908268779759</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3586828/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-00307-817-02-12</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3894911/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>hp-H1KH1PE</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/2952456/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-R030D-189-02-12</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3866200/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>hp-0190017045870</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/2742297/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>russellhobbs-4008496877638</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3610978/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>assmann-4016032439905</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/2990014/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>kingston-0740617298710</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3560888/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>assmann-4016032277897</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3623862/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>seagate-7636490070181</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/2548079/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>teamg-0765441637160</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3601240/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>lenovo-0882861702572</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/1330705/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-FG5KE-288-02-12</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3868510/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>netrack-5908268774600</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3586548/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-M426E-247-02-60</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3870984/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-F40FG-319-02-12</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3894291/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>wd-0718037874937</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3880683/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>msi-4719072448226</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/2521078/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>epson-8715946661803</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3144372/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-F42HF-247-02-12</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/4029051/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>qoltec-5901878521879</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3772099/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>lenovo-0192158407715</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3024417/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>gembird-8716309087681</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3604984/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>logitech-5099206029927</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/1828511/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>goodram-5908267960998</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/4164656/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>lanberg-5901969424737</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3904821/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>logilink-4052792042559</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3614248/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>leitz-0085896723349</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/1477363/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>kingston-0740617308440</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3903814/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>itec-8595611702938</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3372633/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>lanberg-5901969424782</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3904826/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>samsung-8801643802844</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3434647/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>whitenergy-5908214368419</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3621925/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>brother-4977766775762</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/2920048/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>thermaltake-4717964409263</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/2916888/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>logilink-4052792025163</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3611333/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>gigabyte-4719331827847</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/4333639/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-XY4KE-247-02-36</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3872026/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-FG5K1-817-02-36</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3895408/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>netgear-0606449082289</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/1881550/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>gembird-8716309104395</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3641890/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>hp-UB0G6E</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3344889/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>gigabyte-4719331301156</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/2748727/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>hp-HV6Y4E</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/4161756/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC2-10-MNCLD-437-02-12</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/4142007/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>asrock-4710483931161</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3896329/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>hama-4007249892997</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/2388938/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>hp-0725184113994</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/2468686/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>hp-U02C5E</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/4087231/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>lanberg-5901969403640</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3634915/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>gembird-8716309108133</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3643519/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>xiaomi-6941059640011</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3848780/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>kingston-0740617302714</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3796238/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>delock-4043619852048</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/2904047/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>assmann-4016032298496</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/1750416/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>philips-8710103813194</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3644592/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>samsung-8806088677309</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/2898979/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>hp-H9GW7E</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3068989/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>coolingpl-5903018662862</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/4160743/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>blow-5900804070788</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3628902/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>msi-4719072730390</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3901332/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-7K3E1-817-02-60</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3895485/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>delock-4043619847730</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/2564571/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>hp-H9GU8E</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3068817/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>4world-5908214316717</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3588308/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>techly-8057685306127</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3644496/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-F441F-159-02-12</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/4029209/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>lanberg-5901969427486</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/4002116/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>elgato-4260195391710</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3574796/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>logilink-4052792027686</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3611645/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>netrack-5908268776123</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3586689/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>logilink-4052792043709</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3614286/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-V0101-123-02-12</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3871458/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>iiyama-4948570116638</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3309755/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>assmann-4016032390565</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/2827652/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-03981-817-02-12</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3895175/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC5-10-FVHT1-248-02-36</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3870929/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>hp-0193015291119</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3081851/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>art-5901812015532</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3641488/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>hp-G3J30AAE</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/2207141/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>aten-4710423775978</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3608483/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-FG1HE-179-02-12</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3868833/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>hp-H8QP7E</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/2888629/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>coolingpl-5904730204385</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/2625025/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>intel-0675901864039</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/4034665/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-0069F-179-02-12</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/4028869/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>epson-8715946651453</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3082497/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>xerox-0095205832747</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/2663904/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>lanberg-5901969422931</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/4007920/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>hp-0884962554593</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/1713446/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>ubiquiti-0817882020411</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3616282/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>akyga-5901720130525</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3642658/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>siliconpower-4713436133575</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3864967/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>samsung-8801643587628</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3138944/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>verbatim-0023942499763</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/1841797/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>techly-8051128106312</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3644726/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>techly-8051128108705</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/4330422/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>gembird-8716309104296</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3641925/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>asus-4718017286480</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3527009/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>coolingpl-5903018660561</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3855786/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>defender-4714033451246</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3024484/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC5-10-FGVVS-990-02-12</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3870589/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>xerox-0095205841947</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3627582/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-F22HE-928-02-60</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3871374/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>targus-5051794021882</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/2783083/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>itec-8595611703096</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3550901/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>microsoft-0889842594355</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3852543/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>a-data-4710273775845</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3897637/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>gskill-0848354026327</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3658468/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-FE4HF-211-02-12</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3870850/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>gembird-8716309106016</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3643491/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>hp-3S8N8EA#B1R</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/4161913/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-FVM01-813-02-60</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3895622/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-05913-247-02-12</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3868439/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>qoltec-5901878539713</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3656798/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>hp-0191628318599</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/2843411/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>logilink-4260113567159</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3610787/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>lanberg-5901969413830</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3635309/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>asrock-4717677335156</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/3034662/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fortinet-FC-10-FVM04-231-02-12</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/3895453/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>brother-4977766762267</t>
+  </si>
+  <si>
+    <t>https://cby.alsoactebis.com/cop/product/2920052/1432114068334945/datasheet.do</t>
+  </si>
+  <si>
+    <t>fellowes-10043859711380</t>
+  </si>
+  <si>
+    <t>http://cby.alsoactebis.com/cop/product/2016427/1432114068334945/datasheet.do</t>
   </si>
 </sst>
 </file>
@@ -1634,10 +3434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U200"/>
+  <dimension ref="A1:U500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A967" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A975" sqref="A975"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:B500"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3463,6 +5263,2406 @@
         <v>399</v>
       </c>
     </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>400</v>
+      </c>
+      <c r="B201" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>402</v>
+      </c>
+      <c r="B202" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>404</v>
+      </c>
+      <c r="B203" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>406</v>
+      </c>
+      <c r="B204" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>408</v>
+      </c>
+      <c r="B205" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>410</v>
+      </c>
+      <c r="B206" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>412</v>
+      </c>
+      <c r="B207" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>414</v>
+      </c>
+      <c r="B208" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>416</v>
+      </c>
+      <c r="B209" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>418</v>
+      </c>
+      <c r="B210" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>420</v>
+      </c>
+      <c r="B211" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>422</v>
+      </c>
+      <c r="B212" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>424</v>
+      </c>
+      <c r="B213" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>426</v>
+      </c>
+      <c r="B214" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>428</v>
+      </c>
+      <c r="B215" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>430</v>
+      </c>
+      <c r="B216" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>432</v>
+      </c>
+      <c r="B217" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>434</v>
+      </c>
+      <c r="B218" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>436</v>
+      </c>
+      <c r="B219" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>438</v>
+      </c>
+      <c r="B220" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>440</v>
+      </c>
+      <c r="B221" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>442</v>
+      </c>
+      <c r="B222" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>444</v>
+      </c>
+      <c r="B223" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>446</v>
+      </c>
+      <c r="B224" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>448</v>
+      </c>
+      <c r="B225" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>450</v>
+      </c>
+      <c r="B226" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>452</v>
+      </c>
+      <c r="B227" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>454</v>
+      </c>
+      <c r="B228" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>456</v>
+      </c>
+      <c r="B229" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>458</v>
+      </c>
+      <c r="B230" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>460</v>
+      </c>
+      <c r="B231" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>462</v>
+      </c>
+      <c r="B232" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>464</v>
+      </c>
+      <c r="B233" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>466</v>
+      </c>
+      <c r="B234" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>468</v>
+      </c>
+      <c r="B235" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>470</v>
+      </c>
+      <c r="B236" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>472</v>
+      </c>
+      <c r="B237" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>474</v>
+      </c>
+      <c r="B238" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>476</v>
+      </c>
+      <c r="B239" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>478</v>
+      </c>
+      <c r="B240" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>480</v>
+      </c>
+      <c r="B241" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>482</v>
+      </c>
+      <c r="B242" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>484</v>
+      </c>
+      <c r="B243" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>486</v>
+      </c>
+      <c r="B244" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>488</v>
+      </c>
+      <c r="B245" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>490</v>
+      </c>
+      <c r="B246" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>492</v>
+      </c>
+      <c r="B247" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>494</v>
+      </c>
+      <c r="B248" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>496</v>
+      </c>
+      <c r="B249" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>498</v>
+      </c>
+      <c r="B250" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>500</v>
+      </c>
+      <c r="B251" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>502</v>
+      </c>
+      <c r="B252" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>504</v>
+      </c>
+      <c r="B253" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>506</v>
+      </c>
+      <c r="B254" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>508</v>
+      </c>
+      <c r="B255" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>510</v>
+      </c>
+      <c r="B256" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>512</v>
+      </c>
+      <c r="B257" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>514</v>
+      </c>
+      <c r="B258" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>516</v>
+      </c>
+      <c r="B259" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>518</v>
+      </c>
+      <c r="B260" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>520</v>
+      </c>
+      <c r="B261" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>522</v>
+      </c>
+      <c r="B262" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>524</v>
+      </c>
+      <c r="B263" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>526</v>
+      </c>
+      <c r="B264" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>528</v>
+      </c>
+      <c r="B265" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>530</v>
+      </c>
+      <c r="B266" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>532</v>
+      </c>
+      <c r="B267" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>534</v>
+      </c>
+      <c r="B268" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>536</v>
+      </c>
+      <c r="B269" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>538</v>
+      </c>
+      <c r="B270" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>540</v>
+      </c>
+      <c r="B271" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>542</v>
+      </c>
+      <c r="B272" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>544</v>
+      </c>
+      <c r="B273" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>546</v>
+      </c>
+      <c r="B274" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>548</v>
+      </c>
+      <c r="B275" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>550</v>
+      </c>
+      <c r="B276" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>552</v>
+      </c>
+      <c r="B277" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>554</v>
+      </c>
+      <c r="B278" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>556</v>
+      </c>
+      <c r="B279" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>558</v>
+      </c>
+      <c r="B280" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>560</v>
+      </c>
+      <c r="B281" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>562</v>
+      </c>
+      <c r="B282" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>564</v>
+      </c>
+      <c r="B283" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>566</v>
+      </c>
+      <c r="B284" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>568</v>
+      </c>
+      <c r="B285" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>570</v>
+      </c>
+      <c r="B286" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>572</v>
+      </c>
+      <c r="B287" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>574</v>
+      </c>
+      <c r="B288" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>576</v>
+      </c>
+      <c r="B289" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>578</v>
+      </c>
+      <c r="B290" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>580</v>
+      </c>
+      <c r="B291" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>582</v>
+      </c>
+      <c r="B292" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
+        <v>584</v>
+      </c>
+      <c r="B293" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
+        <v>586</v>
+      </c>
+      <c r="B294" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>588</v>
+      </c>
+      <c r="B295" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
+        <v>590</v>
+      </c>
+      <c r="B296" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
+        <v>592</v>
+      </c>
+      <c r="B297" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>594</v>
+      </c>
+      <c r="B298" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
+        <v>596</v>
+      </c>
+      <c r="B299" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A300" t="s">
+        <v>598</v>
+      </c>
+      <c r="B300" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
+        <v>600</v>
+      </c>
+      <c r="B301" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
+        <v>602</v>
+      </c>
+      <c r="B302" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
+        <v>604</v>
+      </c>
+      <c r="B303" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A304" t="s">
+        <v>606</v>
+      </c>
+      <c r="B304" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
+        <v>608</v>
+      </c>
+      <c r="B305" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
+        <v>610</v>
+      </c>
+      <c r="B306" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
+        <v>612</v>
+      </c>
+      <c r="B307" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A308" t="s">
+        <v>614</v>
+      </c>
+      <c r="B308" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
+        <v>616</v>
+      </c>
+      <c r="B309" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A310" t="s">
+        <v>618</v>
+      </c>
+      <c r="B310" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A311" t="s">
+        <v>620</v>
+      </c>
+      <c r="B311" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A312" t="s">
+        <v>622</v>
+      </c>
+      <c r="B312" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A313" t="s">
+        <v>624</v>
+      </c>
+      <c r="B313" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A314" t="s">
+        <v>626</v>
+      </c>
+      <c r="B314" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A315" t="s">
+        <v>628</v>
+      </c>
+      <c r="B315" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A316" t="s">
+        <v>630</v>
+      </c>
+      <c r="B316" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A317" t="s">
+        <v>632</v>
+      </c>
+      <c r="B317" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A318" t="s">
+        <v>634</v>
+      </c>
+      <c r="B318" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A319" t="s">
+        <v>636</v>
+      </c>
+      <c r="B319" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A320" t="s">
+        <v>638</v>
+      </c>
+      <c r="B320" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A321" t="s">
+        <v>640</v>
+      </c>
+      <c r="B321" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A322" t="s">
+        <v>642</v>
+      </c>
+      <c r="B322" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A323" t="s">
+        <v>644</v>
+      </c>
+      <c r="B323" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A324" t="s">
+        <v>646</v>
+      </c>
+      <c r="B324" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A325" t="s">
+        <v>648</v>
+      </c>
+      <c r="B325" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
+        <v>650</v>
+      </c>
+      <c r="B326" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A327" t="s">
+        <v>652</v>
+      </c>
+      <c r="B327" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A328" t="s">
+        <v>654</v>
+      </c>
+      <c r="B328" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A329" t="s">
+        <v>656</v>
+      </c>
+      <c r="B329" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A330" t="s">
+        <v>658</v>
+      </c>
+      <c r="B330" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A331" t="s">
+        <v>660</v>
+      </c>
+      <c r="B331" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A332" t="s">
+        <v>662</v>
+      </c>
+      <c r="B332" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A333" t="s">
+        <v>664</v>
+      </c>
+      <c r="B333" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A334" t="s">
+        <v>666</v>
+      </c>
+      <c r="B334" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A335" t="s">
+        <v>668</v>
+      </c>
+      <c r="B335" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A336" t="s">
+        <v>670</v>
+      </c>
+      <c r="B336" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A337" t="s">
+        <v>672</v>
+      </c>
+      <c r="B337" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A338" t="s">
+        <v>674</v>
+      </c>
+      <c r="B338" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A339" t="s">
+        <v>676</v>
+      </c>
+      <c r="B339" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A340" t="s">
+        <v>678</v>
+      </c>
+      <c r="B340" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A341" t="s">
+        <v>680</v>
+      </c>
+      <c r="B341" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A342" t="s">
+        <v>682</v>
+      </c>
+      <c r="B342" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A343" t="s">
+        <v>684</v>
+      </c>
+      <c r="B343" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A344" t="s">
+        <v>686</v>
+      </c>
+      <c r="B344" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A345" t="s">
+        <v>688</v>
+      </c>
+      <c r="B345" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A346" t="s">
+        <v>690</v>
+      </c>
+      <c r="B346" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A347" t="s">
+        <v>692</v>
+      </c>
+      <c r="B347" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A348" t="s">
+        <v>694</v>
+      </c>
+      <c r="B348" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A349" t="s">
+        <v>696</v>
+      </c>
+      <c r="B349" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A350" t="s">
+        <v>698</v>
+      </c>
+      <c r="B350" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A351" t="s">
+        <v>700</v>
+      </c>
+      <c r="B351" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A352" t="s">
+        <v>702</v>
+      </c>
+      <c r="B352" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A353" t="s">
+        <v>704</v>
+      </c>
+      <c r="B353" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A354" t="s">
+        <v>706</v>
+      </c>
+      <c r="B354" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A355" t="s">
+        <v>708</v>
+      </c>
+      <c r="B355" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A356" t="s">
+        <v>710</v>
+      </c>
+      <c r="B356" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A357" t="s">
+        <v>712</v>
+      </c>
+      <c r="B357" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A358" t="s">
+        <v>714</v>
+      </c>
+      <c r="B358" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A359" t="s">
+        <v>716</v>
+      </c>
+      <c r="B359" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A360" t="s">
+        <v>718</v>
+      </c>
+      <c r="B360" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A361" t="s">
+        <v>720</v>
+      </c>
+      <c r="B361" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A362" t="s">
+        <v>722</v>
+      </c>
+      <c r="B362" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A363" t="s">
+        <v>724</v>
+      </c>
+      <c r="B363" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A364" t="s">
+        <v>726</v>
+      </c>
+      <c r="B364" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A365" t="s">
+        <v>728</v>
+      </c>
+      <c r="B365" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A366" t="s">
+        <v>730</v>
+      </c>
+      <c r="B366" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A367" t="s">
+        <v>732</v>
+      </c>
+      <c r="B367" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A368" t="s">
+        <v>734</v>
+      </c>
+      <c r="B368" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A369" t="s">
+        <v>736</v>
+      </c>
+      <c r="B369" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A370" t="s">
+        <v>738</v>
+      </c>
+      <c r="B370" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A371" t="s">
+        <v>740</v>
+      </c>
+      <c r="B371" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A372" t="s">
+        <v>742</v>
+      </c>
+      <c r="B372" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A373" t="s">
+        <v>744</v>
+      </c>
+      <c r="B373" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A374" t="s">
+        <v>746</v>
+      </c>
+      <c r="B374" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A375" t="s">
+        <v>748</v>
+      </c>
+      <c r="B375" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A376" t="s">
+        <v>750</v>
+      </c>
+      <c r="B376" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A377" t="s">
+        <v>752</v>
+      </c>
+      <c r="B377" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="378" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A378" t="s">
+        <v>754</v>
+      </c>
+      <c r="B378" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="379" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A379" t="s">
+        <v>756</v>
+      </c>
+      <c r="B379" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A380" t="s">
+        <v>758</v>
+      </c>
+      <c r="B380" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="381" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A381" t="s">
+        <v>760</v>
+      </c>
+      <c r="B381" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A382" t="s">
+        <v>762</v>
+      </c>
+      <c r="B382" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A383" t="s">
+        <v>764</v>
+      </c>
+      <c r="B383" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A384" t="s">
+        <v>766</v>
+      </c>
+      <c r="B384" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A385" t="s">
+        <v>768</v>
+      </c>
+      <c r="B385" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="386" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A386" t="s">
+        <v>770</v>
+      </c>
+      <c r="B386" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="387" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A387" t="s">
+        <v>772</v>
+      </c>
+      <c r="B387" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A388" t="s">
+        <v>774</v>
+      </c>
+      <c r="B388" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="389" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A389" t="s">
+        <v>776</v>
+      </c>
+      <c r="B389" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="390" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A390" t="s">
+        <v>778</v>
+      </c>
+      <c r="B390" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="391" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A391" t="s">
+        <v>780</v>
+      </c>
+      <c r="B391" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="392" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A392" t="s">
+        <v>782</v>
+      </c>
+      <c r="B392" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="393" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A393" t="s">
+        <v>784</v>
+      </c>
+      <c r="B393" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="394" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A394" t="s">
+        <v>786</v>
+      </c>
+      <c r="B394" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="395" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A395" t="s">
+        <v>788</v>
+      </c>
+      <c r="B395" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="396" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A396" t="s">
+        <v>790</v>
+      </c>
+      <c r="B396" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="397" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A397" t="s">
+        <v>792</v>
+      </c>
+      <c r="B397" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="398" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A398" t="s">
+        <v>794</v>
+      </c>
+      <c r="B398" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="399" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A399" t="s">
+        <v>796</v>
+      </c>
+      <c r="B399" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="400" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A400" t="s">
+        <v>798</v>
+      </c>
+      <c r="B400" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="401" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A401" t="s">
+        <v>800</v>
+      </c>
+      <c r="B401" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="402" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A402" t="s">
+        <v>802</v>
+      </c>
+      <c r="B402" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="403" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A403" t="s">
+        <v>804</v>
+      </c>
+      <c r="B403" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="404" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A404" t="s">
+        <v>806</v>
+      </c>
+      <c r="B404" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="405" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A405" t="s">
+        <v>808</v>
+      </c>
+      <c r="B405" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="406" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A406" t="s">
+        <v>810</v>
+      </c>
+      <c r="B406" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="407" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A407" t="s">
+        <v>812</v>
+      </c>
+      <c r="B407" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="408" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A408" t="s">
+        <v>814</v>
+      </c>
+      <c r="B408" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="409" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A409" t="s">
+        <v>816</v>
+      </c>
+      <c r="B409" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="410" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A410" t="s">
+        <v>818</v>
+      </c>
+      <c r="B410" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="411" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A411" t="s">
+        <v>820</v>
+      </c>
+      <c r="B411" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="412" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A412" t="s">
+        <v>822</v>
+      </c>
+      <c r="B412" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="413" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A413" t="s">
+        <v>824</v>
+      </c>
+      <c r="B413" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="414" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A414" t="s">
+        <v>826</v>
+      </c>
+      <c r="B414" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="415" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A415" t="s">
+        <v>828</v>
+      </c>
+      <c r="B415" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="416" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A416" t="s">
+        <v>830</v>
+      </c>
+      <c r="B416" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="417" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A417" t="s">
+        <v>832</v>
+      </c>
+      <c r="B417" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="418" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A418" t="s">
+        <v>834</v>
+      </c>
+      <c r="B418" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="419" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A419" t="s">
+        <v>836</v>
+      </c>
+      <c r="B419" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="420" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A420" t="s">
+        <v>838</v>
+      </c>
+      <c r="B420" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="421" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A421" t="s">
+        <v>840</v>
+      </c>
+      <c r="B421" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="422" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A422" t="s">
+        <v>842</v>
+      </c>
+      <c r="B422" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="423" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A423" t="s">
+        <v>844</v>
+      </c>
+      <c r="B423" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="424" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A424" t="s">
+        <v>846</v>
+      </c>
+      <c r="B424" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="425" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A425" t="s">
+        <v>848</v>
+      </c>
+      <c r="B425" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="426" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A426" t="s">
+        <v>850</v>
+      </c>
+      <c r="B426" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="427" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A427" t="s">
+        <v>852</v>
+      </c>
+      <c r="B427" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="428" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A428" t="s">
+        <v>854</v>
+      </c>
+      <c r="B428" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="429" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A429" t="s">
+        <v>856</v>
+      </c>
+      <c r="B429" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="430" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A430" t="s">
+        <v>858</v>
+      </c>
+      <c r="B430" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="431" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A431" t="s">
+        <v>860</v>
+      </c>
+      <c r="B431" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="432" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A432" t="s">
+        <v>862</v>
+      </c>
+      <c r="B432" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="433" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A433" t="s">
+        <v>864</v>
+      </c>
+      <c r="B433" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="434" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A434" t="s">
+        <v>866</v>
+      </c>
+      <c r="B434" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="435" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A435" t="s">
+        <v>868</v>
+      </c>
+      <c r="B435" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="436" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A436" t="s">
+        <v>870</v>
+      </c>
+      <c r="B436" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="437" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A437" t="s">
+        <v>872</v>
+      </c>
+      <c r="B437" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="438" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A438" t="s">
+        <v>874</v>
+      </c>
+      <c r="B438" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="439" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A439" t="s">
+        <v>876</v>
+      </c>
+      <c r="B439" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="440" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A440" t="s">
+        <v>878</v>
+      </c>
+      <c r="B440" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="441" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A441" t="s">
+        <v>880</v>
+      </c>
+      <c r="B441" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="442" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A442" t="s">
+        <v>882</v>
+      </c>
+      <c r="B442" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="443" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A443" t="s">
+        <v>884</v>
+      </c>
+      <c r="B443" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="444" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A444" t="s">
+        <v>886</v>
+      </c>
+      <c r="B444" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="445" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A445" t="s">
+        <v>888</v>
+      </c>
+      <c r="B445" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="446" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A446" t="s">
+        <v>890</v>
+      </c>
+      <c r="B446" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="447" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A447" t="s">
+        <v>892</v>
+      </c>
+      <c r="B447" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="448" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A448" t="s">
+        <v>894</v>
+      </c>
+      <c r="B448" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="449" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A449" t="s">
+        <v>896</v>
+      </c>
+      <c r="B449" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="450" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A450" t="s">
+        <v>898</v>
+      </c>
+      <c r="B450" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="451" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A451" t="s">
+        <v>900</v>
+      </c>
+      <c r="B451" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="452" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A452" t="s">
+        <v>902</v>
+      </c>
+      <c r="B452" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="453" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A453" t="s">
+        <v>904</v>
+      </c>
+      <c r="B453" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="454" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A454" t="s">
+        <v>906</v>
+      </c>
+      <c r="B454" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="455" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A455" t="s">
+        <v>908</v>
+      </c>
+      <c r="B455" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="456" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A456" t="s">
+        <v>910</v>
+      </c>
+      <c r="B456" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="457" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A457" t="s">
+        <v>912</v>
+      </c>
+      <c r="B457" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="458" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A458" t="s">
+        <v>914</v>
+      </c>
+      <c r="B458" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="459" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A459" t="s">
+        <v>916</v>
+      </c>
+      <c r="B459" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="460" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A460" t="s">
+        <v>918</v>
+      </c>
+      <c r="B460" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="461" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A461" t="s">
+        <v>920</v>
+      </c>
+      <c r="B461" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="462" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A462" t="s">
+        <v>922</v>
+      </c>
+      <c r="B462" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="463" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A463" t="s">
+        <v>924</v>
+      </c>
+      <c r="B463" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="464" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A464" t="s">
+        <v>926</v>
+      </c>
+      <c r="B464" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="465" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A465" t="s">
+        <v>928</v>
+      </c>
+      <c r="B465" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="466" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A466" t="s">
+        <v>930</v>
+      </c>
+      <c r="B466" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="467" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A467" t="s">
+        <v>932</v>
+      </c>
+      <c r="B467" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="468" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A468" t="s">
+        <v>934</v>
+      </c>
+      <c r="B468" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="469" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A469" t="s">
+        <v>936</v>
+      </c>
+      <c r="B469" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="470" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A470" t="s">
+        <v>938</v>
+      </c>
+      <c r="B470" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="471" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A471" t="s">
+        <v>940</v>
+      </c>
+      <c r="B471" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="472" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A472" t="s">
+        <v>942</v>
+      </c>
+      <c r="B472" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="473" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A473" t="s">
+        <v>944</v>
+      </c>
+      <c r="B473" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="474" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A474" t="s">
+        <v>946</v>
+      </c>
+      <c r="B474" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="475" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A475" t="s">
+        <v>948</v>
+      </c>
+      <c r="B475" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="476" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A476" t="s">
+        <v>950</v>
+      </c>
+      <c r="B476" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="477" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A477" t="s">
+        <v>952</v>
+      </c>
+      <c r="B477" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="478" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A478" t="s">
+        <v>954</v>
+      </c>
+      <c r="B478" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="479" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A479" t="s">
+        <v>956</v>
+      </c>
+      <c r="B479" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="480" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A480" t="s">
+        <v>958</v>
+      </c>
+      <c r="B480" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="481" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A481" t="s">
+        <v>960</v>
+      </c>
+      <c r="B481" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="482" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A482" t="s">
+        <v>962</v>
+      </c>
+      <c r="B482" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="483" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A483" t="s">
+        <v>964</v>
+      </c>
+      <c r="B483" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="484" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A484" t="s">
+        <v>966</v>
+      </c>
+      <c r="B484" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="485" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A485" t="s">
+        <v>968</v>
+      </c>
+      <c r="B485" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="486" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A486" t="s">
+        <v>970</v>
+      </c>
+      <c r="B486" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="487" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A487" t="s">
+        <v>972</v>
+      </c>
+      <c r="B487" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="488" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A488" t="s">
+        <v>974</v>
+      </c>
+      <c r="B488" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="489" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A489" t="s">
+        <v>976</v>
+      </c>
+      <c r="B489" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="490" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A490" t="s">
+        <v>978</v>
+      </c>
+      <c r="B490" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="491" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A491" t="s">
+        <v>980</v>
+      </c>
+      <c r="B491" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="492" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A492" t="s">
+        <v>982</v>
+      </c>
+      <c r="B492" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="493" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A493" t="s">
+        <v>984</v>
+      </c>
+      <c r="B493" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="494" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A494" t="s">
+        <v>986</v>
+      </c>
+      <c r="B494" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="495" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A495" t="s">
+        <v>988</v>
+      </c>
+      <c r="B495" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="496" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A496" t="s">
+        <v>990</v>
+      </c>
+      <c r="B496" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="497" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A497" t="s">
+        <v>992</v>
+      </c>
+      <c r="B497" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="498" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A498" t="s">
+        <v>994</v>
+      </c>
+      <c r="B498" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="499" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A499" t="s">
+        <v>996</v>
+      </c>
+      <c r="B499" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="500" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A500" t="s">
+        <v>998</v>
+      </c>
+      <c r="B500" t="s">
+        <v>999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>